<commit_message>
FeymanKac and Hotspot results
</commit_message>
<xml_diff>
--- a/rezultati.xlsx
+++ b/rezultati.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Markov folder\Nauka\2024\SICAAI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\.shortcut-targets-by-id\1zct4mxMBZD5OxpOiwMVKqKgJsYsSFZvF\MUPS\SICAAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877910FD-BDD7-4E2C-A663-86A50321C3B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74744B50-EA40-42F9-9C59-053CC906E906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="105" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PiCalc" sheetId="2" r:id="rId1"/>
     <sheet name="Prime" sheetId="1" r:id="rId2"/>
+    <sheet name="Feyman" sheetId="4" r:id="rId3"/>
+    <sheet name="Hotspot" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="15">
   <si>
     <t>prime</t>
   </si>
@@ -55,6 +57,33 @@
   </si>
   <si>
     <t>pi_calc</t>
+  </si>
+  <si>
+    <t>Feyman</t>
+  </si>
+  <si>
+    <t>Hotspot</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 256x256; 8192</t>
+  </si>
+  <si>
+    <t>32x32; 8192</t>
+  </si>
+  <si>
+    <t>1024x1024; 4096</t>
+  </si>
+  <si>
+    <t>1024x1024; 8192</t>
+  </si>
+  <si>
+    <t>1024x1024; 16384</t>
+  </si>
+  <si>
+    <t>1024x1024; 32768</t>
+  </si>
+  <si>
+    <t>omp-task</t>
   </si>
 </sst>
 </file>
@@ -90,8 +119,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1036,6 +1068,1029 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Feyman</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feyman!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>omp</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Feyman!$B$9:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feyman!$B$10:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.3831972522313731</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3727043971227868</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3065597212719626</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2738185346625635</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-17D6-47F1-A6BB-80E014E14A60}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feyman!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>omp_gpt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Feyman!$B$9:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feyman!$B$11:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.7261907890980246</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6981246892376478</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.6486857117003266</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6162836261567288</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-17D6-47F1-A6BB-80E014E14A60}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feyman!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>omp_gpt2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Feyman!$B$9:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feyman!$B$12:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5.2044298409534484</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.2501052434795259</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8482164526563221</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.534021012986365</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-17D6-47F1-A6BB-80E014E14A60}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="633057536"/>
+        <c:axId val="631581040"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="633057536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="631581040"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="631581040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="633057536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Hotspot</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hotspot!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>omp-task</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hotspot!$B$9:$G$9</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>32x32; 8192</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v> 256x256; 8192</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1024x1024; 4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1024x1024; 8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024x1024; 16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024x1024; 32768</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hotspot!$B$10:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.6118747458316387</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.386441123855624</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.6112182586717907</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.6009258578881616</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.6053279912169831</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.2164916308488909</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-88AA-4347-984B-9AF992A6FD39}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hotspot!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>omp_gpt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hotspot!$B$9:$G$9</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>32x32; 8192</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v> 256x256; 8192</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1024x1024; 4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1024x1024; 8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024x1024; 16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024x1024; 32768</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hotspot!$B$11:$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.0123883021933384</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.4472012344365224</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.5834250019509968</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.6339814656926919</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.4822932266723035</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.5127250944805866</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-88AA-4347-984B-9AF992A6FD39}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hotspot!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>omp_gpt2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hotspot!$B$9:$G$9</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>32x32; 8192</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v> 256x256; 8192</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1024x1024; 4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1024x1024; 8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024x1024; 16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024x1024; 32768</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hotspot!$B$12:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.5842993045007594</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6229887964162977</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.6941540466279612</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4044676416479982</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.8485463087524581</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.8783787422129432</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-88AA-4347-984B-9AF992A6FD39}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="633057536"/>
+        <c:axId val="631581040"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="633057536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="631581040"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="631581040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="633057536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1116,6 +2171,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1620,6 +2755,1012 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2190,6 +4331,92 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D629867D-B615-46E7-ACF3-9E75C6F3C32A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="18" name="Chart 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C4CE0E1-6EDD-487C-8411-FFFD6089197C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2471,7 +4698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D2A8F7D-7DEA-487E-8BAD-296E4E4AFFF3}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
@@ -2611,7 +4838,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:D12"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2754,4 +4981,427 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7CF6E27-3BD7-450C-A0F9-DA14AA5BF607}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1000</v>
+      </c>
+      <c r="C2">
+        <v>5000</v>
+      </c>
+      <c r="D2">
+        <v>10000</v>
+      </c>
+      <c r="E2">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>3.0078689999999999</v>
+      </c>
+      <c r="C3">
+        <v>15.052897</v>
+      </c>
+      <c r="D3">
+        <v>29.505106000000001</v>
+      </c>
+      <c r="E3">
+        <v>60.177607999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1.2621150000000001</v>
+      </c>
+      <c r="C4">
+        <v>6.3441939999999999</v>
+      </c>
+      <c r="D4">
+        <v>12.791824</v>
+      </c>
+      <c r="E4">
+        <v>26.465440000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1.1033230000000001</v>
+      </c>
+      <c r="C5">
+        <v>5.5790220000000001</v>
+      </c>
+      <c r="D5">
+        <v>11.139526999999999</v>
+      </c>
+      <c r="E5">
+        <v>23.001179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0.57794400000000001</v>
+      </c>
+      <c r="C6">
+        <v>2.8671609999999998</v>
+      </c>
+      <c r="D6">
+        <v>6.0857650000000003</v>
+      </c>
+      <c r="E6">
+        <v>13.272459</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1000</v>
+      </c>
+      <c r="C9">
+        <v>5000</v>
+      </c>
+      <c r="D9">
+        <v>10000</v>
+      </c>
+      <c r="E9">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <f>B$3/B4</f>
+        <v>2.3831972522313731</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ref="C10:E10" si="0">C$3/C4</f>
+        <v>2.3727043971227868</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>2.3065597212719626</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>2.2738185346625635</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <f t="shared" ref="B11:E12" si="1">B$3/B5</f>
+        <v>2.7261907890980246</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>2.6981246892376478</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>2.6486857117003266</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>2.6162836261567288</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>5.2044298409534484</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>5.2501052434795259</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>4.8482164526563221</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>4.534021012986365</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36DC1CB2-8BB0-4625-9F49-8F20A01971EB}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="7" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1.9817999999999999E-2</v>
+      </c>
+      <c r="C3">
+        <v>1.023747</v>
+      </c>
+      <c r="D3">
+        <v>8.2277629999999995</v>
+      </c>
+      <c r="E3">
+        <v>16.387944999999998</v>
+      </c>
+      <c r="F3">
+        <v>32.910736</v>
+      </c>
+      <c r="G3">
+        <v>66.551295999999994</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>1.2295E-2</v>
+      </c>
+      <c r="C4">
+        <v>0.19006000000000001</v>
+      </c>
+      <c r="D4">
+        <v>1.4663060000000001</v>
+      </c>
+      <c r="E4">
+        <v>2.925935</v>
+      </c>
+      <c r="F4">
+        <v>5.8713309999999996</v>
+      </c>
+      <c r="G4">
+        <v>12.757865000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>9.8480000000000009E-3</v>
+      </c>
+      <c r="C5">
+        <v>0.18794</v>
+      </c>
+      <c r="D5">
+        <v>1.4736050000000001</v>
+      </c>
+      <c r="E5">
+        <v>2.9087679999999998</v>
+      </c>
+      <c r="F5">
+        <v>7.3423879999999997</v>
+      </c>
+      <c r="G5">
+        <v>14.747474</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1.2508999999999999E-2</v>
+      </c>
+      <c r="C6">
+        <v>0.221447</v>
+      </c>
+      <c r="D6">
+        <v>1.7527680000000001</v>
+      </c>
+      <c r="E6">
+        <v>3.720755</v>
+      </c>
+      <c r="F6">
+        <v>8.5514720000000004</v>
+      </c>
+      <c r="G6">
+        <v>17.159566000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <f>B$3/B4</f>
+        <v>1.6118747458316387</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ref="C10:G10" si="0">C$3/C4</f>
+        <v>5.386441123855624</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>5.6112182586717907</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>5.6009258578881616</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>5.6053279912169831</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>5.2164916308488909</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <f t="shared" ref="B11:G12" si="1">B$3/B5</f>
+        <v>2.0123883021933384</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>5.4472012344365224</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>5.5834250019509968</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>5.6339814656926919</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>4.4822932266723035</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>4.5127250944805866</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>1.5842993045007594</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>4.6229887964162977</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>4.6941540466279612</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>4.4044676416479982</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>3.8485463087524581</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>3.8783787422129432</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>